<commit_message>
fixed the pathing for 1
</commit_message>
<xml_diff>
--- a/Testkit/Q1/Environment.xlsx
+++ b/Testkit/Q1/Environment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Casptone Project\TCP_Opertator\Testkit_Operator\Q1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\School\NET\NewQ\Testkit\Q1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E087324F-215A-4BD7-8CC9-C356ABD5A800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18604355-4279-4FDE-9D63-F7A0271BC082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Key</t>
   </si>
@@ -110,15 +110,9 @@
     <t>Database_Password</t>
   </si>
   <si>
-    <t>Khanh@2721</t>
-  </si>
-  <si>
     <t>Default_Database_Name</t>
   </si>
   <si>
-    <t>PE_PRN_Sum25B5_WA</t>
-  </si>
-  <si>
     <t>Default_Database_File_Path</t>
   </si>
   <si>
@@ -219,6 +213,9 @@
   </si>
   <si>
     <t>Meta\Given\Client</t>
+  </si>
+  <si>
+    <t>Library</t>
   </si>
 </sst>
 </file>
@@ -229,7 +226,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -241,7 +238,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -261,7 +258,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -810,17 +807,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="30.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.09765625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -951,69 +948,69 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" s="13"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B18" r:id="rId1" display="Khanh@2721" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1027,107 +1024,107 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="37.21875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="21.69921875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="37.19921875" style="7" customWidth="1"/>
     <col min="3" max="3" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="C2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="C7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -1144,24 +1141,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55852DB-35AC-4970-B37F-1AA8BA374E03}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="18" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="18"/>
+    <col min="2" max="2" width="27.796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.8984375" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="8.8984375" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1169,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>